<commit_message>
inspect adjectives, nouns and numbers
</commit_message>
<xml_diff>
--- a/DOC/schedule.xlsx
+++ b/DOC/schedule.xlsx
@@ -3,14 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C27EFE-06AE-44CA-8C75-5B2CB94B536B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3246E445-68DD-46A7-80BA-DA586BA0A6A1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Task</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,6 +53,58 @@
   </si>
   <si>
     <t>Yusheng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Collect words.
+2. Evaluate the performance of the program.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Collect and test the analyzer.
+2. Help Ahmed evaluate the performance of the analyzer.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Guilde Ahmed to collect what domains words belong to.
+Help Ahmed get familiar with JSON format.
+use this linke "https://www.quora.com/What-is-JSON-2"
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"I would collect Chinese words from China Daily"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Confirm the pattern of the table. Ahmed can supply his collection on the basis of the table.
+The number of the words must be larger the Russian's.
+Ahmed has supplied some examples since last week, inspect the analysis result fo these words and ask Ahmed to evaluate the result.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>We have known word inflection in Arabic: verbs, adjectives, nouns, numbers.
+We have known folding in Arabic: hamza and punctuation.
+Collect examples for verbs, adjective, nouns, numbers
+regular and irregular words
+Collect examples for hamza and punctuation(folding).</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -58,7 +112,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +122,15 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -97,16 +160,16 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -390,228 +453,582 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F53E06D8-87FC-4C0D-80A6-EBD80C98BCAF}">
   <dimension ref="D1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="K1" s="4" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
     </row>
     <row r="4" spans="4:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="K4" s="4" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="K4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D5" s="3"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="4:17" x14ac:dyDescent="0.2">
       <c r="D6" s="3"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="4:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="K7" s="4" t="s">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="K7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
     </row>
     <row r="8" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D8" s="4"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="D9" s="4"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
     </row>
     <row r="11" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="4:17" x14ac:dyDescent="0.2">
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D1:I3"/>
+    <mergeCell ref="K1:Q3"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:I6"/>
+    <mergeCell ref="D7:D9"/>
     <mergeCell ref="K4:K6"/>
     <mergeCell ref="L4:Q6"/>
     <mergeCell ref="E7:I9"/>
     <mergeCell ref="K7:K9"/>
     <mergeCell ref="L7:Q9"/>
-    <mergeCell ref="D1:I3"/>
-    <mergeCell ref="K1:Q3"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="E4:I6"/>
-    <mergeCell ref="D7:D9"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701E0859-5ABC-448C-A5E5-8EE59F3FFD9F}">
+  <dimension ref="B4:R25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="K4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="K23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B4:H19"/>
+    <mergeCell ref="K4:R19"/>
+    <mergeCell ref="B23:H25"/>
+    <mergeCell ref="K23:R25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
prepare to call java method
</commit_message>
<xml_diff>
--- a/DOC/schedule.xlsx
+++ b/DOC/schedule.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47A1976-EC33-4791-9C33-4E5997985B2F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAC828E-BF16-4520-9B16-B68788E5A523}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -413,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701E0859-5ABC-448C-A5E5-8EE59F3FFD9F}">
   <dimension ref="B4:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48:K52"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:Z31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1186,16 +1186,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B48:K52"/>
+    <mergeCell ref="B28:Z31"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B34:N43"/>
+    <mergeCell ref="B33:E33"/>
     <mergeCell ref="B4:H19"/>
     <mergeCell ref="K4:R19"/>
     <mergeCell ref="B23:H25"/>
     <mergeCell ref="K23:R25"/>
     <mergeCell ref="T4:Y19"/>
-    <mergeCell ref="B48:K52"/>
-    <mergeCell ref="B28:Z31"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B34:N43"/>
-    <mergeCell ref="B33:E33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>